<commit_message>
fixed tests for local run
</commit_message>
<xml_diff>
--- a/test/model-rule-data/corrupt.xlsx
+++ b/test/model-rule-data/corrupt.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\oe-cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\evgit\oe-cloud\test\model-rule-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="6405"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="corrupt" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Employee Validation</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>if (HSM &gt; 70) and (SHSM &gt; 70) then true else false</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,11 +202,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -226,6 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +625,9 @@
       <c r="G8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H8" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -632,6 +648,9 @@
       <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="H9" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -652,6 +671,9 @@
       <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="H10" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -671,6 +693,9 @@
       </c>
       <c r="G11" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>